<commit_message>
Updated Excel file inside images_analogy
</commit_message>
<xml_diff>
--- a/images_analogy/30_days_Python_LaxmiPrasannaGandham.xlsx
+++ b/images_analogy/30_days_Python_LaxmiPrasannaGandham.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/ab6b608cdb56ab0f/Desktop/30/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/ab6b608cdb56ab0f/Desktop/30/images_analogy/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="170" documentId="114_{99D204E1-768F-4B65-8764-53DE04542810}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0022EFC5-6CB0-431A-9F2D-706ECA081799}"/>
+  <xr:revisionPtr revIDLastSave="172" documentId="114_{99D204E1-768F-4B65-8764-53DE04542810}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5107860F-E6C7-4FC5-BDC8-4A42DB1D17C4}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{2485688C-545B-4CD8-B98B-95ACB656567E}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="95">
   <si>
     <t xml:space="preserve">               Day </t>
   </si>
@@ -316,6 +316,12 @@
   </si>
   <si>
     <t>https://x.com/LaxmiPrasanna_9/status/1937208257472528856</t>
+  </si>
+  <si>
+    <t>https://tinyurl.com/5d4d59rh</t>
+  </si>
+  <si>
+    <t>https://x.com/LaxmiPrasanna_9/status/1937569931819987432</t>
   </si>
 </sst>
 </file>
@@ -387,10 +393,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -690,10 +692,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0DFD5A1D-9C09-4418-9B53-37F799F9EDDE}">
-  <dimension ref="A1:E28"/>
+  <dimension ref="A1:E29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="H24" sqref="H24"/>
+    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="E33" sqref="E33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1116,6 +1118,14 @@
       </c>
       <c r="E28" s="3" t="s">
         <v>92</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="D29" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="E29" s="3" t="s">
+        <v>94</v>
       </c>
     </row>
   </sheetData>
@@ -1178,8 +1188,10 @@
     <hyperlink ref="E26" r:id="rId50" xr:uid="{3C28C979-965D-4E8C-998B-783F47A42FA2}"/>
     <hyperlink ref="D28" r:id="rId51" xr:uid="{14E47627-E32B-4763-886E-65F3004FFB19}"/>
     <hyperlink ref="E28" r:id="rId52" xr:uid="{F776AC8B-2CC4-4AE5-B023-71123B41999C}"/>
+    <hyperlink ref="D29" r:id="rId53" xr:uid="{1A0DBB4A-F4E5-4D22-AAC2-2169D7CC5217}"/>
+    <hyperlink ref="E29" r:id="rId54" xr:uid="{FC0A03EF-D282-4137-9AB2-CD94290D2525}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId53"/>
+  <pageSetup orientation="portrait" r:id="rId55"/>
 </worksheet>
 </file>
</xml_diff>